<commit_message>
added logic for select * statement
</commit_message>
<xml_diff>
--- a/sample_datasheet.xlsx
+++ b/sample_datasheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2081" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2084" uniqueCount="86">
   <si>
     <t>tc_id</t>
   </si>
@@ -273,6 +273,15 @@
   </si>
   <si>
     <t>ravi</t>
+  </si>
+  <si>
+    <t>10.11</t>
+  </si>
+  <si>
+    <t>333333.22</t>
+  </si>
+  <si>
+    <t>4.jgf</t>
   </si>
 </sst>
 </file>
@@ -594,7 +603,7 @@
   <dimension ref="A1:W206"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -909,8 +918,8 @@
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
+      <c r="A5" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="B5" t="s">
         <v>36</v>
@@ -933,8 +942,8 @@
       <c r="H5" t="s">
         <v>29</v>
       </c>
-      <c r="I5">
-        <v>99.8</v>
+      <c r="I5" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="J5">
         <v>176.6</v>
@@ -1335,8 +1344,8 @@
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>10</v>
+      <c r="A11" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="B11" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
select code is ready and unit tested
</commit_message>
<xml_diff>
--- a/sample_datasheet.xlsx
+++ b/sample_datasheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2084" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2085" uniqueCount="87">
   <si>
     <t>tc_id</t>
   </si>
@@ -282,6 +282,9 @@
   </si>
   <si>
     <t>4.jgf</t>
+  </si>
+  <si>
+    <t>5.jgf</t>
   </si>
 </sst>
 </file>
@@ -603,7 +606,7 @@
   <dimension ref="A1:W206"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,8 +992,8 @@
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
+      <c r="A6" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="B6" t="s">
         <v>36</v>

</xml_diff>